<commit_message>
valores validos y scrollbar para los integrantes de un grupo en asignareva
</commit_message>
<xml_diff>
--- a/api/LibroEstudiantes.xlsx
+++ b/api/LibroEstudiantes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16275" windowHeight="11580"/>
+    <workbookView windowWidth="19635" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <t>Codigo curso</t>
   </si>
   <si>
-    <t>C123O</t>
+    <t>45c</t>
   </si>
   <si>
     <t>Codigo</t>

</xml_diff>